<commit_message>
Populated data organizer and imported to Python
</commit_message>
<xml_diff>
--- a/Data Processing/raw_data/Denmark AMR data organizer JR.xlsx
+++ b/Data Processing/raw_data/Denmark AMR data organizer JR.xlsx
@@ -5,17 +5,20 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\First Analytics\Clients\University of Liverpool\GBADs Github\GBADs-AMU-Dashboard\Data Processing\raw_data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\First Analytics\Clients\University of Liverpool\2023-11 Antimicrobial Usage Revisit\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7027F76-5A6C-43CC-BFD1-453D0770696F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E43C3A2B-B9CC-42CE-AAB3-60E13AB57EF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-3300" yWindow="11890" windowWidth="25820" windowHeight="15500" xr2:uid="{AC3DE23B-CCA8-4C55-A652-BAD7C0A905D8}"/>
+    <workbookView xWindow="-3270" yWindow="11920" windowWidth="25760" windowHeight="15440" activeTab="2" xr2:uid="{AC3DE23B-CCA8-4C55-A652-BAD7C0A905D8}"/>
   </bookViews>
   <sheets>
     <sheet name="Farm summary" sheetId="1" r:id="rId1"/>
     <sheet name="AMR" sheetId="2" r:id="rId2"/>
     <sheet name="AHLE" sheetId="3" r:id="rId3"/>
+    <sheet name="AHLE from U Bern" sheetId="4" r:id="rId4"/>
+    <sheet name="Inputs from U Bern" sheetId="5" r:id="rId5"/>
+    <sheet name="Scenario comps from U Bern" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -43,6 +46,98 @@
     <author>Justin Replogle</author>
   </authors>
   <commentList>
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{05D1D8BF-840B-4ED5-9077-5D2874F852B5}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Justin Replogle:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+This data from file results DANMAP_4Dec.xlsx</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Justin Replogle</author>
+  </authors>
+  <commentList>
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{C996D0C8-ACB5-4CD4-A4CD-3D235034C8AB}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Justin Replogle:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+This data from file results DANMAP_4Dec.xlsx</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Justin Replogle</author>
+  </authors>
+  <commentList>
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{7DDA53E6-1485-4898-BEA9-58A01A7EC072}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Justin Replogle:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+This data from file results DANMAP_4Dec.xlsx</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="C1" authorId="0" shapeId="0" xr:uid="{43C62C6B-1676-4242-AA3E-B03450F54CBB}">
       <text>
         <r>
@@ -71,8 +166,113 @@
 </comments>
 </file>
 
+<file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Justin Replogle</author>
+  </authors>
+  <commentList>
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{361593E7-F749-4283-A85F-D733E490B684}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Justin Replogle:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+From file GBADs_AHLE DK_meeting_20241209.pdf</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments5.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Justin Replogle</author>
+  </authors>
+  <commentList>
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{0FC195DF-7D46-4E20-B099-6D4DA7F62FBD}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Justin Replogle:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+From file GBADs_AHLE DK_meeting_20241209.pdf</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments6.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Justin Replogle</author>
+  </authors>
+  <commentList>
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{3A08CCAD-1774-4D74-B3B5-7024C2F92016}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Justin Replogle:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+From file GBADs_AHLE DK_meeting_20241209.pdf</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="111">
+  <si>
+    <t xml:space="preserve"> farms with sows producing piglets </t>
+  </si>
   <si>
     <t>average of  sows per farm</t>
   </si>
@@ -80,6 +280,9 @@
     <t>average of  weaned piglets per sow per year</t>
   </si>
   <si>
+    <t xml:space="preserve"> farms for weaned pigs</t>
+  </si>
+  <si>
     <t>average pigs produced per year</t>
   </si>
   <si>
@@ -182,25 +385,237 @@
     <t>Production losses</t>
   </si>
   <si>
-    <t>All</t>
-  </si>
-  <si>
-    <t>farms for weaned pigs</t>
-  </si>
-  <si>
-    <t xml:space="preserve">farms with sows producing piglets </t>
+    <t>All?</t>
+  </si>
+  <si>
+    <t>Production stage</t>
+  </si>
+  <si>
+    <t>Number of farms affected</t>
+  </si>
+  <si>
+    <t>Breeding</t>
+  </si>
+  <si>
+    <t>Rearing</t>
+  </si>
+  <si>
+    <t>Fattening</t>
+  </si>
+  <si>
+    <t>TOTAL</t>
+  </si>
+  <si>
+    <t>Stage</t>
+  </si>
+  <si>
+    <t>Variable full name</t>
+  </si>
+  <si>
+    <t>DK-SEGES22-Average</t>
+  </si>
+  <si>
+    <t>DK-SEGES22-Danbred-top5%</t>
+  </si>
+  <si>
+    <t>GBADs Utopia</t>
+  </si>
+  <si>
+    <t>Source</t>
+  </si>
+  <si>
+    <t>breeding</t>
+  </si>
+  <si>
+    <t>Return to estrus rate (%)</t>
+  </si>
+  <si>
+    <t>GBADs default definition</t>
+  </si>
+  <si>
+    <t>Abortions (%)</t>
+  </si>
+  <si>
+    <t>Average piglets born alive per sow per litter</t>
+  </si>
+  <si>
+    <t>PERT Distribution, most likely 2.5% better than Danbred Top5%</t>
+  </si>
+  <si>
+    <t>Average preweaning mortality (%)</t>
+  </si>
+  <si>
+    <t>Average weight of your pigs at weaning (kg)</t>
+  </si>
+  <si>
+    <t>6.3/6.1</t>
+  </si>
+  <si>
+    <t>Same as comparison scenario</t>
+  </si>
+  <si>
+    <t>Litters/sow/year</t>
+  </si>
+  <si>
+    <t>Piglets born alive/sow&amp;year</t>
+  </si>
+  <si>
+    <t>Weaned piglets/sow/year</t>
+  </si>
+  <si>
+    <t>Sow replacement rate</t>
+  </si>
+  <si>
+    <t>nursery</t>
+  </si>
+  <si>
+    <t>Weight at weaning (~ at purchase) (kg)</t>
+  </si>
+  <si>
+    <t>6.4/6.9</t>
+  </si>
+  <si>
+    <t>Average weight of your weaners sold (kg)</t>
+  </si>
+  <si>
+    <t>30.6/32.8</t>
+  </si>
+  <si>
+    <t>Average days of your weaners in nursery</t>
+  </si>
+  <si>
+    <t>44/47</t>
+  </si>
+  <si>
+    <t>Calculated from AGD ideal and "start/end weight" of comparison scenario</t>
+  </si>
+  <si>
+    <t>Mortality in weaners (%)</t>
+  </si>
+  <si>
+    <t>Average feed conversion ratio (FCR) of a healthy weaner until sale</t>
+  </si>
+  <si>
+    <t>ADG weaning to sale (kg)</t>
+  </si>
+  <si>
+    <t>fattening</t>
+  </si>
+  <si>
+    <t>Weight at beginning of fattening period (kg)</t>
+  </si>
+  <si>
+    <t>31.0/33.1</t>
+  </si>
+  <si>
+    <t>Live weight at slaughter (kg)</t>
+  </si>
+  <si>
+    <t>114.7/116.0</t>
+  </si>
+  <si>
+    <t>Average days of fattening until your pigs go to slaughter</t>
+  </si>
+  <si>
+    <t>72/72</t>
+  </si>
+  <si>
+    <t>Mortality in fatteners (%)</t>
+  </si>
+  <si>
+    <t>Average feed conversion ratio (FCR) of a healthy fattener until slaughter</t>
+  </si>
+  <si>
+    <t>ADG fatteners until sale (kg)</t>
+  </si>
+  <si>
+    <t>All columns are differences per year</t>
+  </si>
+  <si>
+    <t>Farm</t>
+  </si>
+  <si>
+    <t>Population</t>
+  </si>
+  <si>
+    <t>Farm type</t>
+  </si>
+  <si>
+    <t>Sows inseminated</t>
+  </si>
+  <si>
+    <t>Piglets born alive</t>
+  </si>
+  <si>
+    <t>Animals In</t>
+  </si>
+  <si>
+    <t>Animals Out</t>
+  </si>
+  <si>
+    <t>Revenue</t>
+  </si>
+  <si>
+    <t>Variable Costs</t>
+  </si>
+  <si>
+    <t>GM</t>
+  </si>
+  <si>
+    <t>delta variable costs / delta GM</t>
+  </si>
+  <si>
+    <t>Working sows needed</t>
+  </si>
+  <si>
+    <t>Farms needed</t>
+  </si>
+  <si>
+    <t>AHLE (AVERAGE - UTOPIA)</t>
+  </si>
+  <si>
+    <t>BREEDING (1000 sows)</t>
+  </si>
+  <si>
+    <t>NURSERY (2500)</t>
+  </si>
+  <si>
+    <t>.</t>
+  </si>
+  <si>
+    <t>FATTENING (2000)</t>
+  </si>
+  <si>
+    <t>Delta GM (AVERAGE - TOP5)</t>
+  </si>
+  <si>
+    <t>Residual loss (TOP5 - UTOPIA)</t>
+  </si>
+  <si>
+    <t>Delta GM per farm</t>
+  </si>
+  <si>
+    <t>Population AHLE median</t>
+  </si>
+  <si>
+    <t>Population AHLE 5% percentile</t>
+  </si>
+  <si>
+    <t>Population AHLE 95% percentile</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="3">
+  <numFmts count="5">
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="_-[$DKK]\ * #,##0.00_-;\-[$DKK]\ * #,##0.00_-;_-[$DKK]\ * &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="166" formatCode="_([$DKK]\ * #,##0.00_);_([$DKK]\ * \(#,##0.00\);_([$DKK]\ * &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="174" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -228,6 +643,33 @@
       <color indexed="81"/>
       <name val="Tahoma"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -262,10 +704,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -274,11 +717,38 @@
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="174" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="5">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+        <u val="double"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+        <u val="double"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+        <u val="double"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -622,11 +1092,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04DCD6B1-487C-4DE3-A34E-C9762E104843}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04DCD6B1-487C-4DE3-A34E-C9762E104843}">
   <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -636,115 +1106,116 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>38</v>
+        <v>0</v>
       </c>
       <c r="B2">
         <v>760</v>
       </c>
       <c r="C2" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B3" s="2">
         <v>824</v>
       </c>
       <c r="C3" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B4" s="2">
         <v>34.1</v>
       </c>
       <c r="C4" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>37</v>
+        <v>3</v>
       </c>
       <c r="B5">
         <v>483</v>
       </c>
       <c r="C5" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B6">
         <v>27105</v>
       </c>
       <c r="C6" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B7">
         <v>1116</v>
       </c>
       <c r="C7" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B8">
         <v>8595</v>
       </c>
       <c r="C8" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B9">
         <f>B7+B5+B2</f>
         <v>2359</v>
       </c>
       <c r="C9" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{066FDB34-4E0C-4994-97D4-A599EB20ADE2}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{066FDB34-4E0C-4994-97D4-A599EB20ADE2}">
   <dimension ref="A1:L10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -759,59 +1230,59 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D1" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="F2" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G2" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="G2" s="1" t="s">
-        <v>30</v>
-      </c>
       <c r="H2" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B3" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C3">
         <v>760</v>
@@ -840,11 +1311,8 @@
       <c r="J3" s="4"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>16</v>
-      </c>
       <c r="B4" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C4">
         <v>483</v>
@@ -873,11 +1341,8 @@
       <c r="J4" s="4"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>16</v>
-      </c>
       <c r="B5" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C5">
         <v>1116</v>
@@ -906,14 +1371,8 @@
       <c r="J5" s="4"/>
     </row>
     <row r="6" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>16</v>
-      </c>
       <c r="B6" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="C6" s="6">
-        <v>2359</v>
+        <v>38</v>
       </c>
       <c r="D6" s="7"/>
       <c r="E6" s="7"/>
@@ -933,10 +1392,10 @@
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B7" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C7">
         <v>760</v>
@@ -965,11 +1424,8 @@
       <c r="L7" s="4"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>17</v>
-      </c>
       <c r="B8" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C8">
         <v>483</v>
@@ -998,11 +1454,8 @@
       <c r="L8" s="4"/>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>17</v>
-      </c>
       <c r="B9" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C9">
         <v>1116</v>
@@ -1031,14 +1484,8 @@
       <c r="L9" s="4"/>
     </row>
     <row r="10" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>17</v>
-      </c>
       <c r="B10" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="C10" s="6">
-        <v>2359</v>
+        <v>38</v>
       </c>
       <c r="J10" s="7">
         <v>191639979.42879176</v>
@@ -1052,11 +1499,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:L14">
-    <cfRule type="expression" dxfId="1" priority="2">
+    <cfRule type="expression" dxfId="4" priority="2">
       <formula>_xlfn.ISFORMULA(A1)</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1064,8 +1512,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C1B6A8A-ED5A-4234-A6FF-DFB5D145238A}">
   <dimension ref="A1:J4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1079,39 +1527,39 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B2">
         <v>760</v>
@@ -1147,7 +1595,7 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B3">
         <v>483</v>
@@ -1183,7 +1631,7 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B4">
         <v>1116</v>
@@ -1219,11 +1667,1033 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:J4">
-    <cfRule type="expression" dxfId="0" priority="2">
+    <cfRule type="expression" dxfId="3" priority="2">
       <formula>_xlfn.ISFORMULA(A1)</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{433F0724-3D99-4B27-A50C-1958F68ED38A}">
+  <dimension ref="A1:F5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25" customWidth="1"/>
+    <col min="4" max="4" width="26.7109375" customWidth="1"/>
+    <col min="5" max="5" width="29.5703125" customWidth="1"/>
+    <col min="6" max="6" width="30.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B2" s="8">
+        <v>774</v>
+      </c>
+      <c r="C2" s="4">
+        <v>4205054</v>
+      </c>
+      <c r="D2" s="4">
+        <v>3253751850</v>
+      </c>
+      <c r="E2" s="4">
+        <v>2981130899</v>
+      </c>
+      <c r="F2" s="4">
+        <v>3532062194</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B3" s="8">
+        <v>911</v>
+      </c>
+      <c r="C3" s="4">
+        <v>694283</v>
+      </c>
+      <c r="D3" s="4">
+        <v>632372102</v>
+      </c>
+      <c r="E3" s="4">
+        <v>600211290</v>
+      </c>
+      <c r="F3" s="4">
+        <v>660741258</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>43</v>
+      </c>
+      <c r="B4" s="8">
+        <v>952</v>
+      </c>
+      <c r="C4" s="4">
+        <v>10757966</v>
+      </c>
+      <c r="D4" s="4">
+        <v>1023891686</v>
+      </c>
+      <c r="E4" s="4">
+        <v>946287109</v>
+      </c>
+      <c r="F4" s="4">
+        <v>1106720036</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B5" s="8">
+        <v>2636</v>
+      </c>
+      <c r="C5" s="8"/>
+      <c r="D5" s="4">
+        <v>4910015637</v>
+      </c>
+      <c r="E5" s="4">
+        <v>4527629298</v>
+      </c>
+      <c r="F5" s="4">
+        <v>5299523488</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="D2:F5">
+    <cfRule type="expression" dxfId="2" priority="2">
+      <formula>_xlfn.ISFORMULA(D2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C2:C4">
+    <cfRule type="expression" dxfId="0" priority="1">
+      <formula>_xlfn.ISFORMULA(C2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2C6A405-1643-47F0-A810-4D471F925852}">
+  <dimension ref="A1:F22"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11" customWidth="1"/>
+    <col min="2" max="2" width="64.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="67.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C2" s="9">
+        <v>5.1999999999999998E-2</v>
+      </c>
+      <c r="D2" s="9">
+        <v>3.9E-2</v>
+      </c>
+      <c r="E2" s="9">
+        <v>0</v>
+      </c>
+      <c r="F2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B3" t="s">
+        <v>54</v>
+      </c>
+      <c r="C3" s="9">
+        <v>2.1000000000000001E-2</v>
+      </c>
+      <c r="D3" s="9">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="E3" s="9">
+        <v>0</v>
+      </c>
+      <c r="F3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>51</v>
+      </c>
+      <c r="B4" t="s">
+        <v>55</v>
+      </c>
+      <c r="C4">
+        <v>18</v>
+      </c>
+      <c r="D4">
+        <v>19.7</v>
+      </c>
+      <c r="E4">
+        <v>20.2</v>
+      </c>
+      <c r="F4" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>51</v>
+      </c>
+      <c r="B5" t="s">
+        <v>57</v>
+      </c>
+      <c r="C5" s="9">
+        <v>0.153</v>
+      </c>
+      <c r="D5" s="9">
+        <v>8.5999999999999993E-2</v>
+      </c>
+      <c r="E5" s="9">
+        <v>0</v>
+      </c>
+      <c r="F5" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>51</v>
+      </c>
+      <c r="B6" t="s">
+        <v>58</v>
+      </c>
+      <c r="C6">
+        <v>6.3</v>
+      </c>
+      <c r="D6">
+        <v>6.1</v>
+      </c>
+      <c r="E6" t="s">
+        <v>59</v>
+      </c>
+      <c r="F6" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>51</v>
+      </c>
+      <c r="B7" t="s">
+        <v>61</v>
+      </c>
+      <c r="C7">
+        <v>2.23</v>
+      </c>
+      <c r="D7">
+        <v>2.33</v>
+      </c>
+      <c r="E7">
+        <v>2.39</v>
+      </c>
+      <c r="F7" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>51</v>
+      </c>
+      <c r="B8" t="s">
+        <v>62</v>
+      </c>
+      <c r="C8">
+        <v>40.1</v>
+      </c>
+      <c r="D8">
+        <v>45.9</v>
+      </c>
+      <c r="E8">
+        <v>47</v>
+      </c>
+      <c r="F8" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>51</v>
+      </c>
+      <c r="B9" t="s">
+        <v>63</v>
+      </c>
+      <c r="C9">
+        <v>34.1</v>
+      </c>
+      <c r="D9">
+        <v>42</v>
+      </c>
+      <c r="E9">
+        <v>47</v>
+      </c>
+      <c r="F9" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>51</v>
+      </c>
+      <c r="B10" t="s">
+        <v>64</v>
+      </c>
+      <c r="C10" s="10">
+        <v>0.54</v>
+      </c>
+      <c r="D10" s="10">
+        <v>0.5</v>
+      </c>
+      <c r="E10" s="10">
+        <v>0.48</v>
+      </c>
+      <c r="F10" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>65</v>
+      </c>
+      <c r="B11" t="s">
+        <v>66</v>
+      </c>
+      <c r="C11">
+        <v>6.4</v>
+      </c>
+      <c r="D11">
+        <v>6.9</v>
+      </c>
+      <c r="E11" t="s">
+        <v>67</v>
+      </c>
+      <c r="F11" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>65</v>
+      </c>
+      <c r="B12" t="s">
+        <v>68</v>
+      </c>
+      <c r="C12">
+        <v>30.6</v>
+      </c>
+      <c r="D12">
+        <v>32.799999999999997</v>
+      </c>
+      <c r="E12" t="s">
+        <v>69</v>
+      </c>
+      <c r="F12" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>65</v>
+      </c>
+      <c r="B13" t="s">
+        <v>70</v>
+      </c>
+      <c r="C13">
+        <v>52</v>
+      </c>
+      <c r="D13">
+        <v>48</v>
+      </c>
+      <c r="E13" t="s">
+        <v>71</v>
+      </c>
+      <c r="F13" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>65</v>
+      </c>
+      <c r="B14" t="s">
+        <v>73</v>
+      </c>
+      <c r="C14" s="9">
+        <v>4.2999999999999997E-2</v>
+      </c>
+      <c r="D14" s="9">
+        <v>0.04</v>
+      </c>
+      <c r="E14" s="9">
+        <v>0</v>
+      </c>
+      <c r="F14" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>65</v>
+      </c>
+      <c r="B15" t="s">
+        <v>74</v>
+      </c>
+      <c r="C15">
+        <v>1.77</v>
+      </c>
+      <c r="D15">
+        <v>1.67</v>
+      </c>
+      <c r="E15">
+        <v>1.63</v>
+      </c>
+      <c r="F15" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>65</v>
+      </c>
+      <c r="B16" t="s">
+        <v>75</v>
+      </c>
+      <c r="C16">
+        <v>0.46500000000000002</v>
+      </c>
+      <c r="D16">
+        <v>0.53900000000000003</v>
+      </c>
+      <c r="E16">
+        <v>0.55200000000000005</v>
+      </c>
+      <c r="F16" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>76</v>
+      </c>
+      <c r="B17" t="s">
+        <v>77</v>
+      </c>
+      <c r="C17">
+        <v>31</v>
+      </c>
+      <c r="D17">
+        <v>33.1</v>
+      </c>
+      <c r="E17" t="s">
+        <v>78</v>
+      </c>
+      <c r="F17" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>76</v>
+      </c>
+      <c r="B18" t="s">
+        <v>79</v>
+      </c>
+      <c r="C18">
+        <v>114.7</v>
+      </c>
+      <c r="D18">
+        <v>116</v>
+      </c>
+      <c r="E18" t="s">
+        <v>80</v>
+      </c>
+      <c r="F18" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>76</v>
+      </c>
+      <c r="B19" t="s">
+        <v>81</v>
+      </c>
+      <c r="C19">
+        <v>81</v>
+      </c>
+      <c r="D19">
+        <v>73</v>
+      </c>
+      <c r="E19" t="s">
+        <v>82</v>
+      </c>
+      <c r="F19" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>76</v>
+      </c>
+      <c r="B20" t="s">
+        <v>83</v>
+      </c>
+      <c r="C20" s="9">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="D20" s="9">
+        <v>3.3000000000000002E-2</v>
+      </c>
+      <c r="E20" s="9">
+        <v>0</v>
+      </c>
+      <c r="F20" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>76</v>
+      </c>
+      <c r="B21" t="s">
+        <v>84</v>
+      </c>
+      <c r="C21">
+        <v>2.65</v>
+      </c>
+      <c r="D21">
+        <v>2.48</v>
+      </c>
+      <c r="E21">
+        <v>2.42</v>
+      </c>
+      <c r="F21" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>76</v>
+      </c>
+      <c r="B22" t="s">
+        <v>85</v>
+      </c>
+      <c r="C22">
+        <v>1.0389999999999999</v>
+      </c>
+      <c r="D22">
+        <v>1.1279999999999999</v>
+      </c>
+      <c r="E22">
+        <v>1.1559999999999999</v>
+      </c>
+      <c r="F22" t="s">
+        <v>56</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FBFC59F0-4538-4121-8D16-983681B04A71}">
+  <dimension ref="A1:L11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L4" sqref="L4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="33" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="28" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A1" s="12" t="s">
+        <v>86</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>100</v>
+      </c>
+      <c r="B3" t="s">
+        <v>101</v>
+      </c>
+      <c r="C3" s="11">
+        <v>170</v>
+      </c>
+      <c r="D3" s="11">
+        <v>-8138</v>
+      </c>
+      <c r="E3" s="11">
+        <v>-14178</v>
+      </c>
+      <c r="F3" s="11">
+        <v>-14178</v>
+      </c>
+      <c r="G3" s="4">
+        <v>-3432870</v>
+      </c>
+      <c r="H3" s="4">
+        <v>764822</v>
+      </c>
+      <c r="I3" s="4">
+        <v>-4205054</v>
+      </c>
+      <c r="J3" s="10">
+        <v>0.18</v>
+      </c>
+      <c r="K3">
+        <v>130431</v>
+      </c>
+      <c r="L3">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>100</v>
+      </c>
+      <c r="B4" t="s">
+        <v>102</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="D4" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="E4" s="11">
+        <v>-8665</v>
+      </c>
+      <c r="F4" s="11">
+        <v>-15644</v>
+      </c>
+      <c r="G4" s="4">
+        <v>-1484920</v>
+      </c>
+      <c r="H4" s="4">
+        <v>-790640</v>
+      </c>
+      <c r="I4" s="4">
+        <v>-694283</v>
+      </c>
+      <c r="J4" s="10">
+        <v>-1.1399999999999999</v>
+      </c>
+      <c r="K4" t="s">
+        <v>103</v>
+      </c>
+      <c r="L4">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>100</v>
+      </c>
+      <c r="B5" t="s">
+        <v>104</v>
+      </c>
+      <c r="C5" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="D5" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="E5" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="F5" s="11">
+        <v>-9298</v>
+      </c>
+      <c r="G5" s="4">
+        <v>-1548074</v>
+      </c>
+      <c r="H5" s="4">
+        <v>-472293</v>
+      </c>
+      <c r="I5" s="4">
+        <v>-1075796</v>
+      </c>
+      <c r="J5" s="10">
+        <v>-0.44</v>
+      </c>
+      <c r="K5" t="s">
+        <v>103</v>
+      </c>
+      <c r="L5">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>105</v>
+      </c>
+      <c r="B6" t="s">
+        <v>101</v>
+      </c>
+      <c r="C6" s="11">
+        <v>43</v>
+      </c>
+      <c r="D6" s="11">
+        <v>-5761</v>
+      </c>
+      <c r="E6" s="11">
+        <v>-7900</v>
+      </c>
+      <c r="F6" s="11">
+        <v>-7900</v>
+      </c>
+      <c r="G6" s="4">
+        <v>-1587024</v>
+      </c>
+      <c r="H6" s="4">
+        <v>746173</v>
+      </c>
+      <c r="I6" s="4">
+        <v>-2333313</v>
+      </c>
+      <c r="J6" s="10">
+        <v>0.32</v>
+      </c>
+      <c r="K6">
+        <v>97116</v>
+      </c>
+      <c r="L6">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>105</v>
+      </c>
+      <c r="B7" t="s">
+        <v>102</v>
+      </c>
+      <c r="C7" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="D7" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="E7" s="11">
+        <v>-4257</v>
+      </c>
+      <c r="F7" s="11">
+        <v>-7686</v>
+      </c>
+      <c r="G7" s="4">
+        <v>-458999</v>
+      </c>
+      <c r="H7" s="4">
+        <v>-3822</v>
+      </c>
+      <c r="I7" s="4">
+        <v>-454872</v>
+      </c>
+      <c r="J7" s="10">
+        <v>-0.01</v>
+      </c>
+      <c r="K7" t="s">
+        <v>103</v>
+      </c>
+      <c r="L7">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>105</v>
+      </c>
+      <c r="B8" t="s">
+        <v>104</v>
+      </c>
+      <c r="C8" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="D8" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="E8" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="F8" s="11">
+        <v>-4153</v>
+      </c>
+      <c r="G8" s="4">
+        <v>-1113831</v>
+      </c>
+      <c r="H8" s="4">
+        <v>-384677</v>
+      </c>
+      <c r="I8" s="4">
+        <v>-729156</v>
+      </c>
+      <c r="J8" s="10">
+        <v>-0.53</v>
+      </c>
+      <c r="K8" t="s">
+        <v>103</v>
+      </c>
+      <c r="L8">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>106</v>
+      </c>
+      <c r="B9" t="s">
+        <v>101</v>
+      </c>
+      <c r="C9" s="11">
+        <v>127</v>
+      </c>
+      <c r="D9" s="11">
+        <v>-2377</v>
+      </c>
+      <c r="E9" s="11">
+        <v>-6278</v>
+      </c>
+      <c r="F9" s="11">
+        <v>-6278</v>
+      </c>
+      <c r="G9" s="4">
+        <v>-1494957</v>
+      </c>
+      <c r="H9" s="4">
+        <v>576140</v>
+      </c>
+      <c r="I9" s="4">
+        <v>-2067488</v>
+      </c>
+      <c r="J9" s="10">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="K9">
+        <v>33316</v>
+      </c>
+      <c r="L9">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>106</v>
+      </c>
+      <c r="B10" t="s">
+        <v>102</v>
+      </c>
+      <c r="C10" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="D10" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="E10" s="11">
+        <v>-4408</v>
+      </c>
+      <c r="F10" s="11">
+        <v>-7958</v>
+      </c>
+      <c r="G10" s="4">
+        <v>-458999</v>
+      </c>
+      <c r="H10" s="4">
+        <v>-3822</v>
+      </c>
+      <c r="I10" s="4">
+        <v>-454872</v>
+      </c>
+      <c r="J10" s="10">
+        <v>-0.01</v>
+      </c>
+      <c r="K10" t="s">
+        <v>103</v>
+      </c>
+      <c r="L10">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>106</v>
+      </c>
+      <c r="B11" t="s">
+        <v>104</v>
+      </c>
+      <c r="C11" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="D11" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="E11" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="F11" s="11">
+        <v>-5145</v>
+      </c>
+      <c r="G11" s="4">
+        <v>-683413</v>
+      </c>
+      <c r="H11" s="4">
+        <v>-114797</v>
+      </c>
+      <c r="I11" s="4">
+        <v>-570417</v>
+      </c>
+      <c r="J11" s="10">
+        <v>-0.2</v>
+      </c>
+      <c r="K11" t="s">
+        <v>103</v>
+      </c>
+      <c r="L11">
+        <v>127</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="G3:I11">
+    <cfRule type="expression" dxfId="1" priority="1">
+      <formula>_xlfn.ISFORMULA(G3)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
DEN AMR percent bars and user controls
</commit_message>
<xml_diff>
--- a/Data Processing/raw_data/Denmark AMR data organizer JR.xlsx
+++ b/Data Processing/raw_data/Denmark AMR data organizer JR.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\First Analytics\Clients\University of Liverpool\2023-11 Antimicrobial Usage Revisit\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D303A46C-E342-4FCD-99B5-AA8486E61A6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5E736D7-AF86-4698-9247-B3B3EF152FA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="2" xr2:uid="{AC3DE23B-CCA8-4C55-A652-BAD7C0A905D8}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="1" xr2:uid="{AC3DE23B-CCA8-4C55-A652-BAD7C0A905D8}"/>
   </bookViews>
   <sheets>
     <sheet name="Farm summary" sheetId="1" r:id="rId1"/>
@@ -269,7 +269,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="112">
   <si>
     <t>average of  sows per farm</t>
   </si>
@@ -599,6 +599,12 @@
   </si>
   <si>
     <t>Total</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Best</t>
   </si>
 </sst>
 </file>
@@ -610,7 +616,7 @@
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="_-[$DKK]\ * #,##0.00_-;\-[$DKK]\ * #,##0.00_-;_-[$DKK]\ * &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="166" formatCode="_([$DKK]\ * #,##0.00_);_([$DKK]\ * \(#,##0.00\);_([$DKK]\ * &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="174" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="167" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="8" x14ac:knownFonts="1">
     <font>
@@ -705,7 +711,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -714,11 +720,12 @@
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="174" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="166" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -1216,10 +1223,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{066FDB34-4E0C-4994-97D4-A599EB20ADE2}">
-  <dimension ref="A1:L10"/>
+  <dimension ref="A1:L14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1292,24 +1299,24 @@
         <f>'Farm summary'!B2</f>
         <v>760</v>
       </c>
-      <c r="D3" s="4">
+      <c r="D3" s="5">
         <v>-8548.6801390308301</v>
       </c>
-      <c r="E3" s="4">
+      <c r="E3" s="5">
         <v>-8993.5832567502948</v>
       </c>
-      <c r="F3" s="4">
+      <c r="F3" s="5">
         <v>-8308.2539107726425</v>
       </c>
-      <c r="G3" s="4">
+      <c r="G3" s="5">
         <f>D3*$C3</f>
         <v>-6496996.9056634307</v>
       </c>
-      <c r="H3" s="4">
+      <c r="H3" s="5">
         <f t="shared" ref="H3:I3" si="0">E3*$C3</f>
         <v>-6835123.2751302244</v>
       </c>
-      <c r="I3" s="4">
+      <c r="I3" s="5">
         <f t="shared" si="0"/>
         <v>-6314272.972187208</v>
       </c>
@@ -1326,24 +1333,24 @@
         <f>'Farm summary'!B5</f>
         <v>483</v>
       </c>
-      <c r="D4" s="4">
+      <c r="D4" s="5">
         <v>-42376.531629593155</v>
       </c>
-      <c r="E4" s="4">
+      <c r="E4" s="5">
         <v>-42376.531629593155</v>
       </c>
-      <c r="F4" s="4">
+      <c r="F4" s="5">
         <v>-42376.531629593155</v>
       </c>
-      <c r="G4" s="4">
+      <c r="G4" s="5">
         <f t="shared" ref="G4:G9" si="1">D4*$C4</f>
         <v>-20467864.777093492</v>
       </c>
-      <c r="H4" s="4">
+      <c r="H4" s="5">
         <f t="shared" ref="H4:H9" si="2">E4*$C4</f>
         <v>-20467864.777093492</v>
       </c>
-      <c r="I4" s="4">
+      <c r="I4" s="5">
         <f t="shared" ref="I4:I9" si="3">F4*$C4</f>
         <v>-20467864.777093492</v>
       </c>
@@ -1360,31 +1367,31 @@
         <f>'Farm summary'!B7</f>
         <v>1116</v>
       </c>
-      <c r="D5" s="4">
+      <c r="D5" s="5">
         <v>0</v>
       </c>
-      <c r="E5" s="4">
+      <c r="E5" s="5">
         <v>0</v>
       </c>
-      <c r="F5" s="4">
+      <c r="F5" s="5">
         <v>0</v>
       </c>
-      <c r="G5" s="4">
+      <c r="G5" s="5">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="H5" s="4">
+      <c r="H5" s="5">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="I5" s="4">
+      <c r="I5" s="5">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="J5" s="4"/>
     </row>
     <row r="6" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="A6" s="6" t="s">
         <v>16</v>
       </c>
       <c r="B6" s="6" t="s">
@@ -1394,18 +1401,18 @@
         <f>SUM(C3:C5)</f>
         <v>2359</v>
       </c>
-      <c r="D6" s="7"/>
-      <c r="E6" s="7"/>
-      <c r="F6" s="7"/>
-      <c r="G6" s="7">
+      <c r="D6" s="13"/>
+      <c r="E6" s="13"/>
+      <c r="F6" s="13"/>
+      <c r="G6" s="13">
         <f>SUM(G3:G5)</f>
         <v>-26964861.682756923</v>
       </c>
-      <c r="H6" s="7">
+      <c r="H6" s="13">
         <f t="shared" ref="H6:I6" si="4">SUM(H3:H5)</f>
         <v>-27302988.052223716</v>
       </c>
-      <c r="I6" s="7">
+      <c r="I6" s="13">
         <f t="shared" si="4"/>
         <v>-26782137.749280699</v>
       </c>
@@ -1430,24 +1437,24 @@
         <f>'Farm summary'!B2</f>
         <v>760</v>
       </c>
-      <c r="D7" s="4">
+      <c r="D7" s="5">
         <v>-192320.20092740544</v>
       </c>
-      <c r="E7" s="4">
+      <c r="E7" s="5">
         <v>-198802.86667517913</v>
       </c>
-      <c r="F7" s="4">
+      <c r="F7" s="5">
         <v>-188817.9891622712</v>
       </c>
-      <c r="G7" s="4">
+      <c r="G7" s="5">
         <f t="shared" si="1"/>
         <v>-146163352.70482814</v>
       </c>
-      <c r="H7" s="4">
+      <c r="H7" s="5">
         <f t="shared" si="2"/>
         <v>-151090178.67313614</v>
       </c>
-      <c r="I7" s="4">
+      <c r="I7" s="5">
         <f t="shared" si="3"/>
         <v>-143501671.76332611</v>
       </c>
@@ -1464,24 +1471,24 @@
         <f>'Farm summary'!B5</f>
         <v>483</v>
       </c>
-      <c r="D8" s="4">
+      <c r="D8" s="5">
         <v>-583624.76948835922</v>
       </c>
-      <c r="E8" s="4">
+      <c r="E8" s="5">
         <v>-583624.76948835922</v>
       </c>
-      <c r="F8" s="4">
+      <c r="F8" s="5">
         <v>-583624.76948835922</v>
       </c>
-      <c r="G8" s="4">
+      <c r="G8" s="5">
         <f t="shared" si="1"/>
         <v>-281890763.6628775</v>
       </c>
-      <c r="H8" s="4">
+      <c r="H8" s="5">
         <f t="shared" si="2"/>
         <v>-281890763.6628775</v>
       </c>
-      <c r="I8" s="4">
+      <c r="I8" s="5">
         <f t="shared" si="3"/>
         <v>-281890763.6628775</v>
       </c>
@@ -1498,31 +1505,31 @@
         <f>'Farm summary'!B7</f>
         <v>1116</v>
       </c>
-      <c r="D9" s="4">
+      <c r="D9" s="5">
         <v>0</v>
       </c>
-      <c r="E9" s="4">
+      <c r="E9" s="5">
         <v>0</v>
       </c>
-      <c r="F9" s="4">
+      <c r="F9" s="5">
         <v>0</v>
       </c>
-      <c r="G9" s="4">
+      <c r="G9" s="5">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="H9" s="4">
+      <c r="H9" s="5">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="I9" s="4">
+      <c r="I9" s="5">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="L9" s="4"/>
     </row>
     <row r="10" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="A10" s="6" t="s">
         <v>17</v>
       </c>
       <c r="B10" s="6" t="s">
@@ -1532,15 +1539,18 @@
         <f>SUM(C7:C9)</f>
         <v>2359</v>
       </c>
-      <c r="G10" s="7">
+      <c r="D10" s="13"/>
+      <c r="E10" s="13"/>
+      <c r="F10" s="13"/>
+      <c r="G10" s="13">
         <f>SUM(G7:G9)</f>
         <v>-428054116.36770564</v>
       </c>
-      <c r="H10" s="7">
+      <c r="H10" s="13">
         <f t="shared" ref="H10:I10" si="5">SUM(H7:H9)</f>
         <v>-432980942.33601367</v>
       </c>
-      <c r="I10" s="7">
+      <c r="I10" s="13">
         <f t="shared" si="5"/>
         <v>-425392435.42620361</v>
       </c>
@@ -1554,9 +1564,144 @@
         <v>428054116.36770564</v>
       </c>
     </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>111</v>
+      </c>
+      <c r="B11" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11">
+        <f>'Farm summary'!B2</f>
+        <v>760</v>
+      </c>
+      <c r="D11" s="5">
+        <f>D3*0.5</f>
+        <v>-4274.3400695154151</v>
+      </c>
+      <c r="E11" s="5">
+        <f t="shared" ref="E11:F11" si="6">E3*0.5</f>
+        <v>-4496.7916283751474</v>
+      </c>
+      <c r="F11" s="5">
+        <f t="shared" si="6"/>
+        <v>-4154.1269553863212</v>
+      </c>
+      <c r="G11" s="5">
+        <f>D11*$C11</f>
+        <v>-3248498.4528317153</v>
+      </c>
+      <c r="H11" s="5">
+        <f t="shared" ref="H11:I11" si="7">E11*$C11</f>
+        <v>-3417561.6375651122</v>
+      </c>
+      <c r="I11" s="5">
+        <f t="shared" si="7"/>
+        <v>-3157136.486093604</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>111</v>
+      </c>
+      <c r="B12" t="s">
+        <v>19</v>
+      </c>
+      <c r="C12">
+        <f>'Farm summary'!B5</f>
+        <v>483</v>
+      </c>
+      <c r="D12" s="5">
+        <f t="shared" ref="D12:F12" si="8">D4*0.5</f>
+        <v>-21188.265814796578</v>
+      </c>
+      <c r="E12" s="5">
+        <f t="shared" si="8"/>
+        <v>-21188.265814796578</v>
+      </c>
+      <c r="F12" s="5">
+        <f t="shared" si="8"/>
+        <v>-21188.265814796578</v>
+      </c>
+      <c r="G12" s="5">
+        <f t="shared" ref="G12:G13" si="9">D12*$C12</f>
+        <v>-10233932.388546746</v>
+      </c>
+      <c r="H12" s="5">
+        <f t="shared" ref="H12:H13" si="10">E12*$C12</f>
+        <v>-10233932.388546746</v>
+      </c>
+      <c r="I12" s="5">
+        <f t="shared" ref="I12:I13" si="11">F12*$C12</f>
+        <v>-10233932.388546746</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>111</v>
+      </c>
+      <c r="B13" t="s">
+        <v>20</v>
+      </c>
+      <c r="C13">
+        <f>'Farm summary'!B7</f>
+        <v>1116</v>
+      </c>
+      <c r="D13" s="5">
+        <f t="shared" ref="D13:F13" si="12">D5*0.5</f>
+        <v>0</v>
+      </c>
+      <c r="E13" s="5">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="F13" s="5">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="G13" s="5">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="H13" s="5">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="I13" s="5">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="C14" s="6">
+        <f>SUM(C11:C13)</f>
+        <v>2359</v>
+      </c>
+      <c r="D14" s="13"/>
+      <c r="E14" s="13"/>
+      <c r="F14" s="13"/>
+      <c r="G14" s="13">
+        <f>SUM(G11:G13)</f>
+        <v>-13482430.841378462</v>
+      </c>
+      <c r="H14" s="13">
+        <f t="shared" ref="H14:I14" si="13">SUM(H11:H13)</f>
+        <v>-13651494.026111858</v>
+      </c>
+      <c r="I14" s="13">
+        <f t="shared" si="13"/>
+        <v>-13391068.874640349</v>
+      </c>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="A1:L14">
-    <cfRule type="expression" dxfId="5" priority="2">
+    <cfRule type="expression" dxfId="0" priority="2">
       <formula>_xlfn.ISFORMULA(A1)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1569,8 +1714,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C1B6A8A-ED5A-4234-A6FF-DFB5D145238A}">
   <dimension ref="A1:J5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1752,13 +1897,13 @@
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A1:J4 A5">
-    <cfRule type="expression" dxfId="4" priority="3">
-      <formula>_xlfn.ISFORMULA(A1)</formula>
+  <conditionalFormatting sqref="A5">
+    <cfRule type="expression" dxfId="5" priority="3">
+      <formula>_xlfn.ISFORMULA(A5)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:J5">
-    <cfRule type="expression" dxfId="0" priority="2">
+    <cfRule type="expression" dxfId="4" priority="2">
       <formula>_xlfn.ISFORMULA(A1)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1884,14 +2029,14 @@
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:F5">
-    <cfRule type="expression" dxfId="3" priority="2">
-      <formula>_xlfn.ISFORMULA(D2)</formula>
+  <conditionalFormatting sqref="C2:C4">
+    <cfRule type="expression" dxfId="3" priority="1">
+      <formula>_xlfn.ISFORMULA(C2)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C2:C4">
-    <cfRule type="expression" dxfId="1" priority="1">
-      <formula>_xlfn.ISFORMULA(C2)</formula>
+  <conditionalFormatting sqref="D2:F5">
+    <cfRule type="expression" dxfId="2" priority="2">
+      <formula>_xlfn.ISFORMULA(D2)</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2581,8 +2726,8 @@
       </c>
       <c r="C7" s="11"/>
       <c r="D7" s="11"/>
-      <c r="E7" s="11">
-        <v>-4257</v>
+      <c r="E7" s="11" t="s">
+        <v>110</v>
       </c>
       <c r="F7" s="11">
         <v>-7686</v>
@@ -2732,7 +2877,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="G3:I11">
-    <cfRule type="expression" dxfId="2" priority="1">
+    <cfRule type="expression" dxfId="1" priority="1">
       <formula>_xlfn.ISFORMULA(G3)</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>